<commit_message>
Calibration: update all scripts to add source info to calibration workbooks
</commit_message>
<xml_diff>
--- a/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
+++ b/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Development\Travel Model One\Calibration\Version 1.5.0\02 Automobile Ownership\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03768B69-7EE7-45F0-A487-114798887C7A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7792575-450E-4588-B541-51F92E16DF7E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="9735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="9735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -626,7 +626,7 @@
     <t>Model Share minus Observed Share</t>
   </si>
   <si>
-    <t>Source: M:\Development\Travel Model One\Calibration\Version 1.5.0\2015_TM150_calib6\OUTPUT\calibration\02_auto_ownership_TM.csv</t>
+    <t>Source:</t>
   </si>
 </sst>
 </file>
@@ -3159,86 +3159,86 @@
       <sheetData sheetId="1">
         <row r="53">
           <cell r="H53">
-            <v>1.1864770474116721</v>
+            <v>1.1818854009146713</v>
           </cell>
           <cell r="J53">
-            <v>-1.0845824267092654</v>
+            <v>-1.1649665084270484</v>
           </cell>
           <cell r="M53">
-            <v>-3.2502311259395973</v>
+            <v>-3.2908417027059005</v>
           </cell>
           <cell r="Q53">
-            <v>-5.312977071472039</v>
+            <v>-5.22933232054113</v>
           </cell>
         </row>
         <row r="54">
           <cell r="H54">
-            <v>0.4258565802249189</v>
+            <v>0.64792389877982692</v>
           </cell>
           <cell r="J54">
-            <v>0.46829606908861432</v>
+            <v>0.58662627332014461</v>
           </cell>
           <cell r="M54">
-            <v>0.14579980750700947</v>
+            <v>0.41307412024275264</v>
           </cell>
           <cell r="Q54">
-            <v>0.14579980750700947</v>
+            <v>-0.26859865029387897</v>
           </cell>
         </row>
         <row r="55">
           <cell r="H55">
-            <v>-0.56599509700263395</v>
+            <v>-0.74518582264347188</v>
           </cell>
           <cell r="J55">
-            <v>-0.44288204546088372</v>
+            <v>-0.59378448636247783</v>
           </cell>
           <cell r="M55">
-            <v>-0.23720985955602231</v>
+            <v>-0.41967084701411378</v>
           </cell>
           <cell r="Q55">
-            <v>-0.23720985955602231</v>
+            <v>-0.31768639292441325</v>
           </cell>
         </row>
         <row r="56">
           <cell r="H56">
-            <v>-0.56599509700263395</v>
+            <v>-0.74518582264347188</v>
           </cell>
           <cell r="J56">
-            <v>-0.44288204546088372</v>
+            <v>-0.59378448636247783</v>
           </cell>
           <cell r="M56">
-            <v>-0.23720985955602231</v>
+            <v>-0.41967084701411378</v>
           </cell>
           <cell r="Q56">
-            <v>-0.23720985955602231</v>
+            <v>-0.31768639292441325</v>
           </cell>
         </row>
         <row r="57">
           <cell r="H57">
-            <v>-0.56599509700263395</v>
+            <v>-0.74518582264347188</v>
           </cell>
           <cell r="J57">
-            <v>-0.44288204546088372</v>
+            <v>-0.59378448636247783</v>
           </cell>
           <cell r="M57">
-            <v>-0.23720985955602231</v>
+            <v>-0.41967084701411378</v>
           </cell>
           <cell r="Q57">
-            <v>-0.23720985955602231</v>
+            <v>-0.31768639292441325</v>
           </cell>
         </row>
         <row r="58">
           <cell r="H58">
-            <v>-0.24341591176276889</v>
+            <v>-0.6595680479649233</v>
           </cell>
           <cell r="J58">
-            <v>0</v>
+            <v>-0.42861162783612095</v>
           </cell>
           <cell r="M58">
-            <v>0</v>
+            <v>-0.41677249145396422</v>
           </cell>
           <cell r="Q58">
-            <v>0</v>
+            <v>-0.40870183229177465</v>
           </cell>
         </row>
       </sheetData>
@@ -3516,6 +3516,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
+    <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:X61"/>
@@ -6248,8 +6249,8 @@
   </sheetPr>
   <dimension ref="B1:N61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6267,7 +6268,7 @@
         <v>185</v>
       </c>
       <c r="J1" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
@@ -6317,19 +6318,19 @@
       </c>
       <c r="D5" s="38">
         <f>'[1]Auto ownership'!H53</f>
-        <v>1.1864770474116721</v>
+        <v>1.1818854009146713</v>
       </c>
       <c r="E5" s="38">
         <f>'[1]Auto ownership'!J53</f>
-        <v>-1.0845824267092654</v>
+        <v>-1.1649665084270484</v>
       </c>
       <c r="F5" s="38">
         <f>'[1]Auto ownership'!M53</f>
-        <v>-3.2502311259395973</v>
+        <v>-3.2908417027059005</v>
       </c>
       <c r="G5" s="38">
         <f>'[1]Auto ownership'!Q53</f>
-        <v>-5.312977071472039</v>
+        <v>-5.22933232054113</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>168</v>
@@ -6364,19 +6365,19 @@
       </c>
       <c r="D6" s="38">
         <f>'[1]Auto ownership'!H54</f>
-        <v>0.4258565802249189</v>
+        <v>0.64792389877982692</v>
       </c>
       <c r="E6" s="38">
         <f>'[1]Auto ownership'!J54</f>
-        <v>0.46829606908861432</v>
+        <v>0.58662627332014461</v>
       </c>
       <c r="F6" s="38">
         <f>'[1]Auto ownership'!M54</f>
-        <v>0.14579980750700947</v>
+        <v>0.41307412024275264</v>
       </c>
       <c r="G6" s="38">
         <f>'[1]Auto ownership'!Q54</f>
-        <v>0.14579980750700947</v>
+        <v>-0.26859865029387897</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>170</v>
@@ -6544,19 +6545,19 @@
       </c>
       <c r="K10" s="25">
         <f>D5</f>
-        <v>1.1864770474116721</v>
+        <v>1.1818854009146713</v>
       </c>
       <c r="L10" s="25">
         <f t="shared" ref="L10:N10" si="2">E5</f>
-        <v>-1.0845824267092654</v>
+        <v>-1.1649665084270484</v>
       </c>
       <c r="M10" s="25">
         <f t="shared" si="2"/>
-        <v>-3.2502311259395973</v>
+        <v>-3.2908417027059005</v>
       </c>
       <c r="N10" s="25">
         <f t="shared" si="2"/>
-        <v>-5.312977071472039</v>
+        <v>-5.22933232054113</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -6568,19 +6569,19 @@
       </c>
       <c r="D11" s="38">
         <f>'[1]Auto ownership'!H55</f>
-        <v>-0.56599509700263395</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="E11" s="38">
         <f>'[1]Auto ownership'!J55</f>
-        <v>-0.44288204546088372</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="F11" s="38">
         <f>'[1]Auto ownership'!M55</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="G11" s="38">
         <f>'[1]Auto ownership'!Q55</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.31768639292441325</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>181</v>
@@ -6590,19 +6591,19 @@
       </c>
       <c r="K11" s="22">
         <f>damp*LN(K5/K6)-damp*LN($J5/$J6)</f>
-        <v>1.1794240149613748</v>
+        <v>0</v>
       </c>
       <c r="L11" s="22">
         <f>damp*LN(L5/L6)-damp*LN($J5/$J6)</f>
-        <v>1.3380598095004033</v>
+        <v>0</v>
       </c>
       <c r="M11" s="22">
         <f>damp*LN(M5/M6)-damp*LN($J5/$J6)</f>
-        <v>0.46264566581682903</v>
+        <v>0</v>
       </c>
       <c r="N11" s="22">
         <f>damp*LN(N5/N6)-damp*LN($J5/$J6)</f>
-        <v>-0.18161520777385043</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -6614,19 +6615,19 @@
       </c>
       <c r="D12" s="38">
         <f>'[1]Auto ownership'!H56</f>
-        <v>-0.56599509700263395</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="E12" s="38">
         <f>'[1]Auto ownership'!J56</f>
-        <v>-0.44288204546088372</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="F12" s="38">
         <f>'[1]Auto ownership'!M56</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="G12" s="38">
         <f>'[1]Auto ownership'!Q56</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.31768639292441325</v>
       </c>
       <c r="I12" s="20" t="s">
         <v>187</v>
@@ -6637,19 +6638,19 @@
       </c>
       <c r="K12" s="23">
         <f>K10+K11</f>
-        <v>2.3659010623730472</v>
+        <v>1.1818854009146713</v>
       </c>
       <c r="L12" s="23">
         <f>L10+L11</f>
-        <v>0.25347738279113785</v>
+        <v>-1.1649665084270484</v>
       </c>
       <c r="M12" s="23">
         <f>M10+M11</f>
-        <v>-2.7875854601227683</v>
+        <v>-3.2908417027059005</v>
       </c>
       <c r="N12" s="23">
         <f>N10+N11</f>
-        <v>-5.4945922792458894</v>
+        <v>-5.22933232054113</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -6661,19 +6662,19 @@
       </c>
       <c r="D13" s="38">
         <f>'[1]Auto ownership'!H57</f>
-        <v>-0.56599509700263395</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="E13" s="38">
         <f>'[1]Auto ownership'!J57</f>
-        <v>-0.44288204546088372</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="F13" s="38">
         <f>'[1]Auto ownership'!M57</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="G13" s="38">
         <f>'[1]Auto ownership'!Q57</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.31768639292441325</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
@@ -6685,19 +6686,19 @@
       </c>
       <c r="D14" s="39">
         <f>'[1]Auto ownership'!H58</f>
-        <v>-0.24341591176276889</v>
+        <v>-0.6595680479649233</v>
       </c>
       <c r="E14" s="39">
         <f>'[1]Auto ownership'!J58</f>
-        <v>0</v>
+        <v>-0.42861162783612095</v>
       </c>
       <c r="F14" s="39">
         <f>'[1]Auto ownership'!M58</f>
-        <v>0</v>
+        <v>-0.41677249145396422</v>
       </c>
       <c r="G14" s="39">
         <f>'[1]Auto ownership'!Q58</f>
-        <v>0</v>
+        <v>-0.40870183229177465</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -6747,19 +6748,19 @@
       </c>
       <c r="D18" s="38">
         <f>K12</f>
-        <v>2.3659010623730472</v>
+        <v>1.1818854009146713</v>
       </c>
       <c r="E18" s="38">
         <f>L12</f>
-        <v>0.25347738279113785</v>
+        <v>-1.1649665084270484</v>
       </c>
       <c r="F18" s="38">
         <f>M12</f>
-        <v>-2.7875854601227683</v>
+        <v>-3.2908417027059005</v>
       </c>
       <c r="G18" s="38">
         <f>N12</f>
-        <v>-5.4945922792458894</v>
+        <v>-5.22933232054113</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>168</v>
@@ -6794,19 +6795,19 @@
       </c>
       <c r="D19" s="38">
         <f>K25</f>
-        <v>-0.45762506149317506</v>
+        <v>0.64792389877982692</v>
       </c>
       <c r="E19" s="38">
         <f>L25</f>
-        <v>-1.2522563874919879</v>
+        <v>0.58662627332014461</v>
       </c>
       <c r="F19" s="38">
         <f>M25</f>
-        <v>-1.9925841862663738</v>
+        <v>0.41307412024275264</v>
       </c>
       <c r="G19" s="38">
         <f>N25</f>
-        <v>-2.5140003765603294</v>
+        <v>-0.26859865029387897</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>170</v>
@@ -6971,19 +6972,19 @@
       </c>
       <c r="K23" s="25">
         <f>D6</f>
-        <v>0.4258565802249189</v>
+        <v>0.64792389877982692</v>
       </c>
       <c r="L23" s="25">
         <f>E6</f>
-        <v>0.46829606908861432</v>
+        <v>0.58662627332014461</v>
       </c>
       <c r="M23" s="25">
         <f>F6</f>
-        <v>0.14579980750700947</v>
+        <v>0.41307412024275264</v>
       </c>
       <c r="N23" s="25">
         <f>G6</f>
-        <v>0.14579980750700947</v>
+        <v>-0.26859865029387897</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
@@ -6996,19 +6997,19 @@
       </c>
       <c r="D24" s="38">
         <f>K37</f>
-        <v>-6.5429747618583889E-3</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="E24" s="38">
         <f>L37</f>
-        <v>0.2142829812712832</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="F24" s="38">
         <f>M37</f>
-        <v>0.5670572201482329</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="G24" s="38">
         <f>N37</f>
-        <v>0.41729424794442233</v>
+        <v>-0.31768639292441325</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>181</v>
@@ -7018,19 +7019,19 @@
       </c>
       <c r="K24" s="22">
         <f>damp*LN(K18/K19)-damp*LN($J18/$J19)-K11</f>
-        <v>-0.88348164171809396</v>
+        <v>0</v>
       </c>
       <c r="L24" s="22">
         <f>damp*LN(L18/L19)-damp*LN($J18/$J19)-L11</f>
-        <v>-1.7205524565806023</v>
+        <v>0</v>
       </c>
       <c r="M24" s="22">
         <f>damp*LN(M18/M19)-damp*LN($J18/$J19)-M11</f>
-        <v>-2.1383839937733833</v>
+        <v>0</v>
       </c>
       <c r="N24" s="22">
         <f>damp*LN(N18/N19)-damp*LN($J18/$J19)</f>
-        <v>-2.6598001840673389</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
@@ -7043,19 +7044,19 @@
       </c>
       <c r="D25" s="38">
         <f>K37</f>
-        <v>-6.5429747618583889E-3</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="E25" s="38">
         <f>L37</f>
-        <v>0.2142829812712832</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="F25" s="38">
         <f>M37</f>
-        <v>0.5670572201482329</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="G25" s="38">
         <f>N37</f>
-        <v>0.41729424794442233</v>
+        <v>-0.31768639292441325</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>187</v>
@@ -7066,19 +7067,19 @@
       </c>
       <c r="K25" s="23">
         <f>K23+K24</f>
-        <v>-0.45762506149317506</v>
+        <v>0.64792389877982692</v>
       </c>
       <c r="L25" s="23">
         <f>L23+L24</f>
-        <v>-1.2522563874919879</v>
+        <v>0.58662627332014461</v>
       </c>
       <c r="M25" s="23">
         <f>M23+M24</f>
-        <v>-1.9925841862663738</v>
+        <v>0.41307412024275264</v>
       </c>
       <c r="N25" s="23">
         <f>N23+N24</f>
-        <v>-2.5140003765603294</v>
+        <v>-0.26859865029387897</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
@@ -7091,19 +7092,19 @@
       </c>
       <c r="D26" s="38">
         <f>K37</f>
-        <v>-6.5429747618583889E-3</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="E26" s="38">
         <f>L37</f>
-        <v>0.2142829812712832</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="F26" s="38">
         <f>M37</f>
-        <v>0.5670572201482329</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="G26" s="38">
         <f>N37</f>
-        <v>0.41729424794442233</v>
+        <v>-0.31768639292441325</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
@@ -7115,19 +7116,19 @@
       </c>
       <c r="D27" s="39">
         <f>K49</f>
-        <v>0.48241742641422125</v>
+        <v>-0.6595680479649233</v>
       </c>
       <c r="E27" s="39">
         <f t="shared" ref="E27:G27" si="3">L49</f>
-        <v>0.75944426660480358</v>
+        <v>-0.42861162783612095</v>
       </c>
       <c r="F27" s="39">
         <f t="shared" si="3"/>
-        <v>0.6850851826575366</v>
+        <v>-0.41677249145396422</v>
       </c>
       <c r="G27" s="39">
         <f t="shared" si="3"/>
-        <v>0.41096648660527557</v>
+        <v>-0.40870183229177465</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
@@ -7266,19 +7267,19 @@
       </c>
       <c r="K35" s="25">
         <f>D12</f>
-        <v>-0.56599509700263395</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="L35" s="25">
         <f>E12</f>
-        <v>-0.44288204546088372</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="M35" s="25">
         <f>F12</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="N35" s="25">
         <f>G12</f>
-        <v>-0.23720985955602231</v>
+        <v>-0.31768639292441325</v>
       </c>
     </row>
     <row r="36" spans="9:14" x14ac:dyDescent="0.2">
@@ -7290,19 +7291,19 @@
       </c>
       <c r="K36" s="22">
         <f>damp*LN(K30/K31)-damp*LN($J30/$J31)-K11</f>
-        <v>0.55945212224077556</v>
+        <v>0</v>
       </c>
       <c r="L36" s="22">
         <f>damp*LN(L30/L31)-damp*LN($J30/$J31)-L11</f>
-        <v>0.65716502673216692</v>
+        <v>0</v>
       </c>
       <c r="M36" s="22">
         <f>damp*LN(M30/M31)-damp*LN($J30/$J31)-M11</f>
-        <v>0.80426707970425526</v>
+        <v>0</v>
       </c>
       <c r="N36" s="22">
         <f>damp*LN(N30/N31)-damp*LN($J30/$J31)</f>
-        <v>0.65450410750044463</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="9:14" x14ac:dyDescent="0.2">
@@ -7315,19 +7316,19 @@
       </c>
       <c r="K37" s="23">
         <f>K35+K36</f>
-        <v>-6.5429747618583889E-3</v>
+        <v>-0.74518582264347188</v>
       </c>
       <c r="L37" s="23">
         <f>L35+L36</f>
-        <v>0.2142829812712832</v>
+        <v>-0.59378448636247783</v>
       </c>
       <c r="M37" s="23">
         <f>M35+M36</f>
-        <v>0.5670572201482329</v>
+        <v>-0.41967084701411378</v>
       </c>
       <c r="N37" s="23">
         <f>N35+N36</f>
-        <v>0.41729424794442233</v>
+        <v>-0.31768639292441325</v>
       </c>
     </row>
     <row r="41" spans="9:14" x14ac:dyDescent="0.2">
@@ -7466,19 +7467,19 @@
       </c>
       <c r="K47" s="25">
         <f>D14</f>
-        <v>-0.24341591176276889</v>
+        <v>-0.6595680479649233</v>
       </c>
       <c r="L47" s="25">
         <f>E14</f>
-        <v>0</v>
+        <v>-0.42861162783612095</v>
       </c>
       <c r="M47" s="25">
         <f>F14</f>
-        <v>0</v>
+        <v>-0.41677249145396422</v>
       </c>
       <c r="N47" s="25">
         <f>G14</f>
-        <v>0</v>
+        <v>-0.40870183229177465</v>
       </c>
     </row>
     <row r="48" spans="9:14" x14ac:dyDescent="0.2">
@@ -7490,19 +7491,19 @@
       </c>
       <c r="K48" s="22">
         <f>damp*LN(K42/K43)-damp*LN($J42/$J43)-K11</f>
-        <v>0.72583333817699014</v>
+        <v>0</v>
       </c>
       <c r="L48" s="22">
         <f>damp*LN(L42/L43)-damp*LN($J42/$J43)-L11</f>
-        <v>0.75944426660480358</v>
+        <v>0</v>
       </c>
       <c r="M48" s="22">
         <f>damp*LN(M42/M43)-damp*LN($J42/$J43)-M11</f>
-        <v>0.6850851826575366</v>
+        <v>0</v>
       </c>
       <c r="N48" s="22">
         <f>damp*LN(N42/N43)-damp*LN($J42/$J43)-N11</f>
-        <v>0.41096648660527557</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="9:14" x14ac:dyDescent="0.2">
@@ -7515,19 +7516,19 @@
       </c>
       <c r="K49" s="23">
         <f>K47+K48</f>
-        <v>0.48241742641422125</v>
+        <v>-0.6595680479649233</v>
       </c>
       <c r="L49" s="23">
         <f>L47+L48</f>
-        <v>0.75944426660480358</v>
+        <v>-0.42861162783612095</v>
       </c>
       <c r="M49" s="23">
         <f>M47+M48</f>
-        <v>0.6850851826575366</v>
+        <v>-0.41677249145396422</v>
       </c>
       <c r="N49" s="23">
         <f>N47+N48</f>
-        <v>0.41096648660527557</v>
+        <v>-0.40870183229177465</v>
       </c>
     </row>
     <row r="52" spans="9:14" x14ac:dyDescent="0.2">
@@ -7693,19 +7694,19 @@
       </c>
       <c r="K60" s="22">
         <f>damp*LN(K54/K55)-damp*LN($J54/$J55)-K11</f>
-        <v>0.51559738460454985</v>
+        <v>0</v>
       </c>
       <c r="L60" s="22">
         <f>damp*LN(L54/L55)-damp*LN($J54/$J55)-L11</f>
-        <v>0.74982343063473356</v>
+        <v>0</v>
       </c>
       <c r="M60" s="22">
         <f>damp*LN(M54/M55)-damp*LN($J54/$J55)-M11</f>
-        <v>0.74006706480674511</v>
+        <v>0</v>
       </c>
       <c r="N60" s="22">
         <f>-damp*LN($J54/$J55)</f>
-        <v>1.3736707707247826</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="9:14" x14ac:dyDescent="0.2">
@@ -7718,19 +7719,19 @@
       </c>
       <c r="K61" s="23">
         <f>K59+K60</f>
-        <v>0.51559738460454985</v>
+        <v>0</v>
       </c>
       <c r="L61" s="23">
         <f>L59+L60</f>
-        <v>0.74982343063473356</v>
+        <v>0</v>
       </c>
       <c r="M61" s="23">
         <f>M59+M60</f>
-        <v>0.74006706480674511</v>
+        <v>0</v>
       </c>
       <c r="N61" s="23">
         <f>N59+N60</f>
-        <v>1.3736707707247826</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7778,8 +7779,8 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Formatting updates to calibration workbook
</commit_message>
<xml_diff>
--- a/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
+++ b/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Development\Travel Model One\Calibration\Version 1.5.0\02 Automobile Ownership\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-calib1.5.2\utilities\calibration\workbook_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7C9DBF-839F-48DB-B49A-758BB23717A0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849DFD70-D4F0-445C-B52A-F3A2C67CCF14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="3210" windowWidth="21600" windowHeight="7050" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12255" yWindow="2175" windowWidth="22305" windowHeight="11745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -3146,98 +3146,98 @@
       <sheetName val="Calibration (3 futures)"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="53">
           <cell r="H53">
-            <v>1.1194866301814053</v>
+            <v>1.1128706549904406</v>
           </cell>
           <cell r="J53">
-            <v>-1.2528378912699398</v>
+            <v>-1.262829694334757</v>
           </cell>
           <cell r="M53">
-            <v>-3.3908387334512509</v>
+            <v>-3.3985810003028987</v>
           </cell>
           <cell r="Q53">
-            <v>-5.3341016107731933</v>
+            <v>-5.3571199709700137</v>
           </cell>
         </row>
         <row r="54">
           <cell r="H54">
-            <v>0.56439548580637522</v>
+            <v>0.56063073772732686</v>
           </cell>
           <cell r="J54">
-            <v>0.5379554735176848</v>
+            <v>0.55153411191094204</v>
           </cell>
           <cell r="M54">
-            <v>0.39092463437753017</v>
+            <v>0.350838403703571</v>
           </cell>
           <cell r="Q54">
-            <v>-0.22954551623730995</v>
+            <v>-0.25337040289458285</v>
           </cell>
         </row>
         <row r="55">
           <cell r="H55">
-            <v>-0.59719691043545919</v>
+            <v>-0.5634652620087649</v>
           </cell>
           <cell r="J55">
-            <v>-0.4227416056224364</v>
+            <v>-0.39739096404853719</v>
           </cell>
           <cell r="M55">
-            <v>-0.23596437414065086</v>
+            <v>-0.20145009515535278</v>
           </cell>
           <cell r="Q55">
-            <v>-0.10702209611476492</v>
+            <v>-6.2140580452059467E-2</v>
           </cell>
         </row>
         <row r="56">
           <cell r="H56">
-            <v>-0.59719691043545919</v>
+            <v>-0.5634652620087649</v>
           </cell>
           <cell r="J56">
-            <v>-0.4227416056224364</v>
+            <v>-0.39739096404853719</v>
           </cell>
           <cell r="M56">
-            <v>-0.23596437414065086</v>
+            <v>-0.20145009515535278</v>
           </cell>
           <cell r="Q56">
-            <v>-0.10702209611476492</v>
+            <v>-6.2140580452059467E-2</v>
           </cell>
         </row>
         <row r="57">
           <cell r="H57">
-            <v>-0.59719691043545919</v>
+            <v>-0.5634652620087649</v>
           </cell>
           <cell r="J57">
-            <v>-0.4227416056224364</v>
+            <v>-0.39739096404853719</v>
           </cell>
           <cell r="M57">
-            <v>-0.23596437414065086</v>
+            <v>-0.20145009515535278</v>
           </cell>
           <cell r="Q57">
-            <v>-0.10702209611476492</v>
+            <v>-6.2140580452059467E-2</v>
           </cell>
         </row>
         <row r="58">
           <cell r="H58">
-            <v>-0.43807538815243918</v>
+            <v>-0.4199239375559411</v>
           </cell>
           <cell r="J58">
-            <v>-0.19396329257023737</v>
+            <v>-0.18316132003964297</v>
           </cell>
           <cell r="M58">
-            <v>-0.18861355666776683</v>
+            <v>-0.12420569703097233</v>
           </cell>
           <cell r="Q58">
-            <v>-0.12036201193254809</v>
+            <v>-0.15034195392335276</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6204,8 +6204,8 @@
   </sheetPr>
   <dimension ref="B1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6273,19 +6273,19 @@
       </c>
       <c r="D5" s="33">
         <f>'[1]Auto ownership'!H53</f>
-        <v>1.1194866301814053</v>
+        <v>1.1128706549904406</v>
       </c>
       <c r="E5" s="33">
         <f>'[1]Auto ownership'!J53</f>
-        <v>-1.2528378912699398</v>
+        <v>-1.262829694334757</v>
       </c>
       <c r="F5" s="33">
         <f>'[1]Auto ownership'!M53</f>
-        <v>-3.3908387334512509</v>
+        <v>-3.3985810003028987</v>
       </c>
       <c r="G5" s="33">
         <f>'[1]Auto ownership'!Q53</f>
-        <v>-5.3341016107731933</v>
+        <v>-5.3571199709700137</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>168</v>
@@ -6320,19 +6320,19 @@
       </c>
       <c r="D6" s="33">
         <f>'[1]Auto ownership'!H54</f>
-        <v>0.56439548580637522</v>
+        <v>0.56063073772732686</v>
       </c>
       <c r="E6" s="33">
         <f>'[1]Auto ownership'!J54</f>
-        <v>0.5379554735176848</v>
+        <v>0.55153411191094204</v>
       </c>
       <c r="F6" s="33">
         <f>'[1]Auto ownership'!M54</f>
-        <v>0.39092463437753017</v>
+        <v>0.350838403703571</v>
       </c>
       <c r="G6" s="33">
         <f>'[1]Auto ownership'!Q54</f>
-        <v>-0.22954551623730995</v>
+        <v>-0.25337040289458285</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>170</v>
@@ -6500,19 +6500,19 @@
       </c>
       <c r="K10" s="23">
         <f>D5</f>
-        <v>1.1194866301814053</v>
+        <v>1.1128706549904406</v>
       </c>
       <c r="L10" s="23">
         <f t="shared" ref="L10:N10" si="2">E5</f>
-        <v>-1.2528378912699398</v>
+        <v>-1.262829694334757</v>
       </c>
       <c r="M10" s="23">
         <f t="shared" si="2"/>
-        <v>-3.3908387334512509</v>
+        <v>-3.3985810003028987</v>
       </c>
       <c r="N10" s="23">
         <f t="shared" si="2"/>
-        <v>-5.3341016107731933</v>
+        <v>-5.3571199709700137</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -6524,19 +6524,19 @@
       </c>
       <c r="D11" s="33">
         <f>'[1]Auto ownership'!H55</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="E11" s="33">
         <f>'[1]Auto ownership'!J55</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="F11" s="33">
         <f>'[1]Auto ownership'!M55</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="G11" s="33">
         <f>'[1]Auto ownership'!Q55</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>181</v>
@@ -6570,19 +6570,19 @@
       </c>
       <c r="D12" s="33">
         <f>'[1]Auto ownership'!H56</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="E12" s="33">
         <f>'[1]Auto ownership'!J56</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="F12" s="33">
         <f>'[1]Auto ownership'!M56</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="G12" s="33">
         <f>'[1]Auto ownership'!Q56</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>187</v>
@@ -6593,19 +6593,19 @@
       </c>
       <c r="K12" s="21">
         <f>K10+K11</f>
-        <v>1.1194866301814053</v>
+        <v>1.1128706549904406</v>
       </c>
       <c r="L12" s="21">
         <f>L10+L11</f>
-        <v>-1.2528378912699398</v>
+        <v>-1.262829694334757</v>
       </c>
       <c r="M12" s="21">
         <f>M10+M11</f>
-        <v>-3.3908387334512509</v>
+        <v>-3.3985810003028987</v>
       </c>
       <c r="N12" s="21">
         <f>N10+N11</f>
-        <v>-5.3341016107731933</v>
+        <v>-5.3571199709700137</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -6617,19 +6617,19 @@
       </c>
       <c r="D13" s="33">
         <f>'[1]Auto ownership'!H57</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="E13" s="33">
         <f>'[1]Auto ownership'!J57</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="F13" s="33">
         <f>'[1]Auto ownership'!M57</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="G13" s="33">
         <f>'[1]Auto ownership'!Q57</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
@@ -6641,19 +6641,19 @@
       </c>
       <c r="D14" s="34">
         <f>'[1]Auto ownership'!H58</f>
-        <v>-0.43807538815243918</v>
+        <v>-0.4199239375559411</v>
       </c>
       <c r="E14" s="34">
         <f>'[1]Auto ownership'!J58</f>
-        <v>-0.19396329257023737</v>
+        <v>-0.18316132003964297</v>
       </c>
       <c r="F14" s="34">
         <f>'[1]Auto ownership'!M58</f>
-        <v>-0.18861355666776683</v>
+        <v>-0.12420569703097233</v>
       </c>
       <c r="G14" s="34">
         <f>'[1]Auto ownership'!Q58</f>
-        <v>-0.12036201193254809</v>
+        <v>-0.15034195392335276</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -6703,19 +6703,19 @@
       </c>
       <c r="D18" s="33">
         <f>K12</f>
-        <v>1.1194866301814053</v>
+        <v>1.1128706549904406</v>
       </c>
       <c r="E18" s="33">
         <f>L12</f>
-        <v>-1.2528378912699398</v>
+        <v>-1.262829694334757</v>
       </c>
       <c r="F18" s="33">
         <f>M12</f>
-        <v>-3.3908387334512509</v>
+        <v>-3.3985810003028987</v>
       </c>
       <c r="G18" s="33">
         <f>N12</f>
-        <v>-5.3341016107731933</v>
+        <v>-5.3571199709700137</v>
       </c>
       <c r="I18" s="22" t="s">
         <v>168</v>
@@ -6750,19 +6750,19 @@
       </c>
       <c r="D19" s="33">
         <f>K25</f>
-        <v>0.56439548580637522</v>
+        <v>0.56063073772732686</v>
       </c>
       <c r="E19" s="33">
         <f>L25</f>
-        <v>0.5379554735176848</v>
+        <v>0.55153411191094204</v>
       </c>
       <c r="F19" s="33">
         <f>M25</f>
-        <v>0.39092463437753017</v>
+        <v>0.350838403703571</v>
       </c>
       <c r="G19" s="33">
         <f>N25</f>
-        <v>-0.22954551623730995</v>
+        <v>-0.25337040289458285</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>170</v>
@@ -6927,19 +6927,19 @@
       </c>
       <c r="K23" s="23">
         <f>D6</f>
-        <v>0.56439548580637522</v>
+        <v>0.56063073772732686</v>
       </c>
       <c r="L23" s="23">
         <f>E6</f>
-        <v>0.5379554735176848</v>
+        <v>0.55153411191094204</v>
       </c>
       <c r="M23" s="23">
         <f>F6</f>
-        <v>0.39092463437753017</v>
+        <v>0.350838403703571</v>
       </c>
       <c r="N23" s="23">
         <f>G6</f>
-        <v>-0.22954551623730995</v>
+        <v>-0.25337040289458285</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
@@ -6952,19 +6952,19 @@
       </c>
       <c r="D24" s="33">
         <f>K37</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="E24" s="33">
         <f>L37</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="F24" s="33">
         <f>M37</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="G24" s="33">
         <f>N37</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>181</v>
@@ -6999,19 +6999,19 @@
       </c>
       <c r="D25" s="33">
         <f>K37</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="E25" s="33">
         <f>L37</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="F25" s="33">
         <f>M37</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="G25" s="33">
         <f>N37</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>187</v>
@@ -7022,19 +7022,19 @@
       </c>
       <c r="K25" s="21">
         <f>K23+K24</f>
-        <v>0.56439548580637522</v>
+        <v>0.56063073772732686</v>
       </c>
       <c r="L25" s="21">
         <f>L23+L24</f>
-        <v>0.5379554735176848</v>
+        <v>0.55153411191094204</v>
       </c>
       <c r="M25" s="21">
         <f>M23+M24</f>
-        <v>0.39092463437753017</v>
+        <v>0.350838403703571</v>
       </c>
       <c r="N25" s="21">
         <f>N23+N24</f>
-        <v>-0.22954551623730995</v>
+        <v>-0.25337040289458285</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
@@ -7047,19 +7047,19 @@
       </c>
       <c r="D26" s="33">
         <f>K37</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="E26" s="33">
         <f>L37</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="F26" s="33">
         <f>M37</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="G26" s="33">
         <f>N37</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
@@ -7071,19 +7071,19 @@
       </c>
       <c r="D27" s="34">
         <f>K49</f>
-        <v>-0.43807538815243918</v>
+        <v>-0.4199239375559411</v>
       </c>
       <c r="E27" s="34">
         <f t="shared" ref="E27:G27" si="3">L49</f>
-        <v>-0.19396329257023737</v>
+        <v>-0.18316132003964297</v>
       </c>
       <c r="F27" s="34">
         <f t="shared" si="3"/>
-        <v>-0.18861355666776683</v>
+        <v>-0.12420569703097233</v>
       </c>
       <c r="G27" s="34">
         <f t="shared" si="3"/>
-        <v>-0.12036201193254809</v>
+        <v>-0.15034195392335276</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
@@ -7222,19 +7222,19 @@
       </c>
       <c r="K35" s="23">
         <f>D12</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="L35" s="23">
         <f>E12</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="M35" s="23">
         <f>F12</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="N35" s="23">
         <f>G12</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
     </row>
     <row r="36" spans="9:14" x14ac:dyDescent="0.2">
@@ -7271,19 +7271,19 @@
       </c>
       <c r="K37" s="21">
         <f>K35+K36</f>
-        <v>-0.59719691043545919</v>
+        <v>-0.5634652620087649</v>
       </c>
       <c r="L37" s="21">
         <f>L35+L36</f>
-        <v>-0.4227416056224364</v>
+        <v>-0.39739096404853719</v>
       </c>
       <c r="M37" s="21">
         <f>M35+M36</f>
-        <v>-0.23596437414065086</v>
+        <v>-0.20145009515535278</v>
       </c>
       <c r="N37" s="21">
         <f>N35+N36</f>
-        <v>-0.10702209611476492</v>
+        <v>-6.2140580452059467E-2</v>
       </c>
     </row>
     <row r="41" spans="9:14" x14ac:dyDescent="0.2">
@@ -7422,19 +7422,19 @@
       </c>
       <c r="K47" s="23">
         <f>D14</f>
-        <v>-0.43807538815243918</v>
+        <v>-0.4199239375559411</v>
       </c>
       <c r="L47" s="23">
         <f>E14</f>
-        <v>-0.19396329257023737</v>
+        <v>-0.18316132003964297</v>
       </c>
       <c r="M47" s="23">
         <f>F14</f>
-        <v>-0.18861355666776683</v>
+        <v>-0.12420569703097233</v>
       </c>
       <c r="N47" s="23">
         <f>G14</f>
-        <v>-0.12036201193254809</v>
+        <v>-0.15034195392335276</v>
       </c>
     </row>
     <row r="48" spans="9:14" x14ac:dyDescent="0.2">
@@ -7471,19 +7471,19 @@
       </c>
       <c r="K49" s="21">
         <f>K47+K48</f>
-        <v>-0.43807538815243918</v>
+        <v>-0.4199239375559411</v>
       </c>
       <c r="L49" s="21">
         <f>L47+L48</f>
-        <v>-0.19396329257023737</v>
+        <v>-0.18316132003964297</v>
       </c>
       <c r="M49" s="21">
         <f>M47+M48</f>
-        <v>-0.18861355666776683</v>
+        <v>-0.12420569703097233</v>
       </c>
       <c r="N49" s="21">
         <f>N47+N48</f>
-        <v>-0.12036201193254809</v>
+        <v>-0.15034195392335276</v>
       </c>
     </row>
     <row r="52" spans="9:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
AutoOwnership Santa Clara constant
</commit_message>
<xml_diff>
--- a/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
+++ b/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-calib1.5.2\utilities\calibration\workbook_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849DFD70-D4F0-445C-B52A-F3A2C67CCF14}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE30C9E3-DBC8-42EE-BA48-6F81490DE103}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12255" yWindow="2175" windowWidth="22305" windowHeight="11745" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="1830" windowWidth="23025" windowHeight="14370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -1335,7 +1335,17 @@
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="6" tint="-0.24994659260841701"/>
@@ -3146,98 +3156,98 @@
       <sheetName val="Calibration (3 futures)"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="53">
           <cell r="H53">
-            <v>1.1128706549904406</v>
+            <v>1.1169201775500097</v>
           </cell>
           <cell r="J53">
-            <v>-1.262829694334757</v>
+            <v>-1.2581644773938045</v>
           </cell>
           <cell r="M53">
-            <v>-3.3985810003028987</v>
+            <v>-3.3920136409186741</v>
           </cell>
           <cell r="Q53">
-            <v>-5.3571199709700137</v>
+            <v>-5.3456796840622633</v>
           </cell>
         </row>
         <row r="54">
           <cell r="H54">
-            <v>0.56063073772732686</v>
+            <v>0.57577284999430334</v>
           </cell>
           <cell r="J54">
-            <v>0.55153411191094204</v>
+            <v>0.55366202552278654</v>
           </cell>
           <cell r="M54">
-            <v>0.350838403703571</v>
+            <v>0.38682074249887466</v>
           </cell>
           <cell r="Q54">
-            <v>-0.25337040289458285</v>
+            <v>-0.1894468159171615</v>
           </cell>
         </row>
         <row r="55">
           <cell r="H55">
-            <v>-0.5634652620087649</v>
+            <v>-0.57634490091114654</v>
           </cell>
           <cell r="J55">
-            <v>-0.39739096404853719</v>
+            <v>-0.39584972567051246</v>
           </cell>
           <cell r="M55">
-            <v>-0.20145009515535278</v>
+            <v>-0.20585904713356956</v>
           </cell>
           <cell r="Q55">
-            <v>-6.2140580452059467E-2</v>
+            <v>-4.232053272803607E-2</v>
           </cell>
         </row>
         <row r="56">
           <cell r="H56">
-            <v>-0.5634652620087649</v>
+            <v>-0.57634490091114654</v>
           </cell>
           <cell r="J56">
-            <v>-0.39739096404853719</v>
+            <v>-0.39584972567051246</v>
           </cell>
           <cell r="M56">
-            <v>-0.20145009515535278</v>
+            <v>-0.20585904713356956</v>
           </cell>
           <cell r="Q56">
-            <v>-6.2140580452059467E-2</v>
+            <v>-4.232053272803607E-2</v>
           </cell>
         </row>
         <row r="57">
           <cell r="H57">
-            <v>-0.5634652620087649</v>
+            <v>-0.57634490091114654</v>
           </cell>
           <cell r="J57">
-            <v>-0.39739096404853719</v>
+            <v>-0.39584972567051246</v>
           </cell>
           <cell r="M57">
-            <v>-0.20145009515535278</v>
+            <v>-0.20585904713356956</v>
           </cell>
           <cell r="Q57">
-            <v>-6.2140580452059467E-2</v>
+            <v>-4.232053272803607E-2</v>
           </cell>
         </row>
         <row r="58">
           <cell r="H58">
-            <v>-0.4199239375559411</v>
+            <v>-0.43165170650309287</v>
           </cell>
           <cell r="J58">
-            <v>-0.18316132003964297</v>
+            <v>-0.18439159511209577</v>
           </cell>
           <cell r="M58">
-            <v>-0.12420569703097233</v>
+            <v>-0.15794956039873473</v>
           </cell>
           <cell r="Q58">
-            <v>-0.15034195392335276</v>
+            <v>-0.13889887457587119</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6204,8 +6214,8 @@
   </sheetPr>
   <dimension ref="B1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6273,19 +6283,19 @@
       </c>
       <c r="D5" s="33">
         <f>'[1]Auto ownership'!H53</f>
-        <v>1.1128706549904406</v>
+        <v>1.1169201775500097</v>
       </c>
       <c r="E5" s="33">
         <f>'[1]Auto ownership'!J53</f>
-        <v>-1.262829694334757</v>
+        <v>-1.2581644773938045</v>
       </c>
       <c r="F5" s="33">
         <f>'[1]Auto ownership'!M53</f>
-        <v>-3.3985810003028987</v>
+        <v>-3.3920136409186741</v>
       </c>
       <c r="G5" s="33">
         <f>'[1]Auto ownership'!Q53</f>
-        <v>-5.3571199709700137</v>
+        <v>-5.3456796840622633</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>168</v>
@@ -6320,19 +6330,19 @@
       </c>
       <c r="D6" s="33">
         <f>'[1]Auto ownership'!H54</f>
-        <v>0.56063073772732686</v>
+        <v>0.57577284999430334</v>
       </c>
       <c r="E6" s="33">
         <f>'[1]Auto ownership'!J54</f>
-        <v>0.55153411191094204</v>
+        <v>0.55366202552278654</v>
       </c>
       <c r="F6" s="33">
         <f>'[1]Auto ownership'!M54</f>
-        <v>0.350838403703571</v>
+        <v>0.38682074249887466</v>
       </c>
       <c r="G6" s="33">
         <f>'[1]Auto ownership'!Q54</f>
-        <v>-0.25337040289458285</v>
+        <v>-0.1894468159171615</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>170</v>
@@ -6500,19 +6510,19 @@
       </c>
       <c r="K10" s="23">
         <f>D5</f>
-        <v>1.1128706549904406</v>
+        <v>1.1169201775500097</v>
       </c>
       <c r="L10" s="23">
         <f t="shared" ref="L10:N10" si="2">E5</f>
-        <v>-1.262829694334757</v>
+        <v>-1.2581644773938045</v>
       </c>
       <c r="M10" s="23">
         <f t="shared" si="2"/>
-        <v>-3.3985810003028987</v>
+        <v>-3.3920136409186741</v>
       </c>
       <c r="N10" s="23">
         <f t="shared" si="2"/>
-        <v>-5.3571199709700137</v>
+        <v>-5.3456796840622633</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -6524,19 +6534,19 @@
       </c>
       <c r="D11" s="33">
         <f>'[1]Auto ownership'!H55</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="E11" s="33">
         <f>'[1]Auto ownership'!J55</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="F11" s="33">
         <f>'[1]Auto ownership'!M55</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="G11" s="33">
         <f>'[1]Auto ownership'!Q55</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>181</v>
@@ -6570,19 +6580,19 @@
       </c>
       <c r="D12" s="33">
         <f>'[1]Auto ownership'!H56</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="E12" s="33">
         <f>'[1]Auto ownership'!J56</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="F12" s="33">
         <f>'[1]Auto ownership'!M56</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="G12" s="33">
         <f>'[1]Auto ownership'!Q56</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>187</v>
@@ -6593,19 +6603,19 @@
       </c>
       <c r="K12" s="21">
         <f>K10+K11</f>
-        <v>1.1128706549904406</v>
+        <v>1.1169201775500097</v>
       </c>
       <c r="L12" s="21">
         <f>L10+L11</f>
-        <v>-1.262829694334757</v>
+        <v>-1.2581644773938045</v>
       </c>
       <c r="M12" s="21">
         <f>M10+M11</f>
-        <v>-3.3985810003028987</v>
+        <v>-3.3920136409186741</v>
       </c>
       <c r="N12" s="21">
         <f>N10+N11</f>
-        <v>-5.3571199709700137</v>
+        <v>-5.3456796840622633</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -6617,19 +6627,19 @@
       </c>
       <c r="D13" s="33">
         <f>'[1]Auto ownership'!H57</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="E13" s="33">
         <f>'[1]Auto ownership'!J57</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="F13" s="33">
         <f>'[1]Auto ownership'!M57</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="G13" s="33">
         <f>'[1]Auto ownership'!Q57</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
@@ -6641,19 +6651,19 @@
       </c>
       <c r="D14" s="34">
         <f>'[1]Auto ownership'!H58</f>
-        <v>-0.4199239375559411</v>
+        <v>-0.43165170650309287</v>
       </c>
       <c r="E14" s="34">
         <f>'[1]Auto ownership'!J58</f>
-        <v>-0.18316132003964297</v>
+        <v>-0.18439159511209577</v>
       </c>
       <c r="F14" s="34">
         <f>'[1]Auto ownership'!M58</f>
-        <v>-0.12420569703097233</v>
+        <v>-0.15794956039873473</v>
       </c>
       <c r="G14" s="34">
         <f>'[1]Auto ownership'!Q58</f>
-        <v>-0.15034195392335276</v>
+        <v>-0.13889887457587119</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -6703,19 +6713,19 @@
       </c>
       <c r="D18" s="33">
         <f>K12</f>
-        <v>1.1128706549904406</v>
+        <v>1.1169201775500097</v>
       </c>
       <c r="E18" s="33">
         <f>L12</f>
-        <v>-1.262829694334757</v>
+        <v>-1.2581644773938045</v>
       </c>
       <c r="F18" s="33">
         <f>M12</f>
-        <v>-3.3985810003028987</v>
+        <v>-3.3920136409186741</v>
       </c>
       <c r="G18" s="33">
         <f>N12</f>
-        <v>-5.3571199709700137</v>
+        <v>-5.3456796840622633</v>
       </c>
       <c r="I18" s="22" t="s">
         <v>168</v>
@@ -6750,19 +6760,19 @@
       </c>
       <c r="D19" s="33">
         <f>K25</f>
-        <v>0.56063073772732686</v>
+        <v>0.57577284999430334</v>
       </c>
       <c r="E19" s="33">
         <f>L25</f>
-        <v>0.55153411191094204</v>
+        <v>0.55366202552278654</v>
       </c>
       <c r="F19" s="33">
         <f>M25</f>
-        <v>0.350838403703571</v>
+        <v>0.38682074249887466</v>
       </c>
       <c r="G19" s="33">
         <f>N25</f>
-        <v>-0.25337040289458285</v>
+        <v>-0.1894468159171615</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>170</v>
@@ -6839,16 +6849,20 @@
         <f>J61</f>
         <v>0</v>
       </c>
-      <c r="D21" s="24">
-        <v>0</v>
-      </c>
-      <c r="E21" s="24">
-        <v>0</v>
-      </c>
-      <c r="F21" s="24">
-        <v>0</v>
-      </c>
-      <c r="G21" s="24">
+      <c r="D21" s="33">
+        <f>K61</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="33">
+        <f t="shared" ref="E21:G21" si="3">L61</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="33">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I21" s="18" t="s">
@@ -6927,19 +6941,19 @@
       </c>
       <c r="K23" s="23">
         <f>D6</f>
-        <v>0.56063073772732686</v>
+        <v>0.57577284999430334</v>
       </c>
       <c r="L23" s="23">
         <f>E6</f>
-        <v>0.55153411191094204</v>
+        <v>0.55366202552278654</v>
       </c>
       <c r="M23" s="23">
         <f>F6</f>
-        <v>0.350838403703571</v>
+        <v>0.38682074249887466</v>
       </c>
       <c r="N23" s="23">
         <f>G6</f>
-        <v>-0.25337040289458285</v>
+        <v>-0.1894468159171615</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
@@ -6952,19 +6966,19 @@
       </c>
       <c r="D24" s="33">
         <f>K37</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="E24" s="33">
         <f>L37</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="F24" s="33">
         <f>M37</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="G24" s="33">
         <f>N37</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>181</v>
@@ -6999,19 +7013,19 @@
       </c>
       <c r="D25" s="33">
         <f>K37</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="E25" s="33">
         <f>L37</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="F25" s="33">
         <f>M37</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="G25" s="33">
         <f>N37</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>187</v>
@@ -7022,19 +7036,19 @@
       </c>
       <c r="K25" s="21">
         <f>K23+K24</f>
-        <v>0.56063073772732686</v>
+        <v>0.57577284999430334</v>
       </c>
       <c r="L25" s="21">
         <f>L23+L24</f>
-        <v>0.55153411191094204</v>
+        <v>0.55366202552278654</v>
       </c>
       <c r="M25" s="21">
         <f>M23+M24</f>
-        <v>0.350838403703571</v>
+        <v>0.38682074249887466</v>
       </c>
       <c r="N25" s="21">
         <f>N23+N24</f>
-        <v>-0.25337040289458285</v>
+        <v>-0.1894468159171615</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
@@ -7047,19 +7061,19 @@
       </c>
       <c r="D26" s="33">
         <f>K37</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="E26" s="33">
         <f>L37</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="F26" s="33">
         <f>M37</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="G26" s="33">
         <f>N37</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
@@ -7071,19 +7085,19 @@
       </c>
       <c r="D27" s="34">
         <f>K49</f>
-        <v>-0.4199239375559411</v>
+        <v>-0.43165170650309287</v>
       </c>
       <c r="E27" s="34">
-        <f t="shared" ref="E27:G27" si="3">L49</f>
-        <v>-0.18316132003964297</v>
+        <f t="shared" ref="E27:G27" si="4">L49</f>
+        <v>-0.18439159511209577</v>
       </c>
       <c r="F27" s="34">
-        <f t="shared" si="3"/>
-        <v>-0.12420569703097233</v>
+        <f t="shared" si="4"/>
+        <v>-0.15794956039873473</v>
       </c>
       <c r="G27" s="34">
-        <f t="shared" si="3"/>
-        <v>-0.15034195392335276</v>
+        <f t="shared" si="4"/>
+        <v>-0.13889887457587119</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
@@ -7222,19 +7236,19 @@
       </c>
       <c r="K35" s="23">
         <f>D12</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="L35" s="23">
         <f>E12</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="M35" s="23">
         <f>F12</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="N35" s="23">
         <f>G12</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
     </row>
     <row r="36" spans="9:14" x14ac:dyDescent="0.2">
@@ -7271,19 +7285,19 @@
       </c>
       <c r="K37" s="21">
         <f>K35+K36</f>
-        <v>-0.5634652620087649</v>
+        <v>-0.57634490091114654</v>
       </c>
       <c r="L37" s="21">
         <f>L35+L36</f>
-        <v>-0.39739096404853719</v>
+        <v>-0.39584972567051246</v>
       </c>
       <c r="M37" s="21">
         <f>M35+M36</f>
-        <v>-0.20145009515535278</v>
+        <v>-0.20585904713356956</v>
       </c>
       <c r="N37" s="21">
         <f>N35+N36</f>
-        <v>-6.2140580452059467E-2</v>
+        <v>-4.232053272803607E-2</v>
       </c>
     </row>
     <row r="41" spans="9:14" x14ac:dyDescent="0.2">
@@ -7422,19 +7436,19 @@
       </c>
       <c r="K47" s="23">
         <f>D14</f>
-        <v>-0.4199239375559411</v>
+        <v>-0.43165170650309287</v>
       </c>
       <c r="L47" s="23">
         <f>E14</f>
-        <v>-0.18316132003964297</v>
+        <v>-0.18439159511209577</v>
       </c>
       <c r="M47" s="23">
         <f>F14</f>
-        <v>-0.12420569703097233</v>
+        <v>-0.15794956039873473</v>
       </c>
       <c r="N47" s="23">
         <f>G14</f>
-        <v>-0.15034195392335276</v>
+        <v>-0.13889887457587119</v>
       </c>
     </row>
     <row r="48" spans="9:14" x14ac:dyDescent="0.2">
@@ -7471,19 +7485,19 @@
       </c>
       <c r="K49" s="21">
         <f>K47+K48</f>
-        <v>-0.4199239375559411</v>
+        <v>-0.43165170650309287</v>
       </c>
       <c r="L49" s="21">
         <f>L47+L48</f>
-        <v>-0.18316132003964297</v>
+        <v>-0.18439159511209577</v>
       </c>
       <c r="M49" s="21">
         <f>M47+M48</f>
-        <v>-0.12420569703097233</v>
+        <v>-0.15794956039873473</v>
       </c>
       <c r="N49" s="21">
         <f>N47+N48</f>
-        <v>-0.15034195392335276</v>
+        <v>-0.13889887457587119</v>
       </c>
     </row>
     <row r="52" spans="9:14" x14ac:dyDescent="0.2">
@@ -7660,7 +7674,7 @@
         <v>0</v>
       </c>
       <c r="N60" s="20">
-        <f>-damp*LN($J54/$J55)</f>
+        <f>damp*LN(N54/N55)-damp*LN($J54/$J55)-N11</f>
         <v>0</v>
       </c>
     </row>
@@ -7691,6 +7705,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:G6">
+    <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:G14">
     <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7698,7 +7720,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:G14">
+  <conditionalFormatting sqref="D18:G19">
     <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7706,7 +7728,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:G19">
+  <conditionalFormatting sqref="D24:G27">
     <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7714,7 +7736,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:G27">
+  <conditionalFormatting sqref="D21:G21">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix missing update to Santa Clara constant in AutoOwnership calib template
</commit_message>
<xml_diff>
--- a/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
+++ b/utilities/calibration/workbook_templates/02_AutoOwnership_blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-calib1.5.2\utilities\calibration\workbook_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE30C9E3-DBC8-42EE-BA48-6F81490DE103}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D89494F-8D4C-4809-B281-DC55F0EC2E40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="1830" windowWidth="23025" windowHeight="14370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11310" yWindow="6150" windowWidth="25725" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="3" r:id="rId1"/>
@@ -1335,7 +1335,17 @@
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="16" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="6" tint="-0.24994659260841701"/>
@@ -3156,98 +3166,112 @@
       <sheetName val="Calibration (3 futures)"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="53">
           <cell r="H53">
-            <v>1.1169201775500097</v>
+            <v>1.1172992162790916</v>
           </cell>
           <cell r="J53">
-            <v>-1.2581644773938045</v>
+            <v>-1.2565051850306308</v>
           </cell>
           <cell r="M53">
-            <v>-3.3920136409186741</v>
+            <v>-3.3877106944960214</v>
           </cell>
           <cell r="Q53">
-            <v>-5.3456796840622633</v>
+            <v>-5.3502031433147499</v>
           </cell>
         </row>
         <row r="54">
           <cell r="H54">
-            <v>0.57577284999430334</v>
+            <v>0.57931801393948956</v>
           </cell>
           <cell r="J54">
-            <v>0.55366202552278654</v>
+            <v>0.56301198136124597</v>
           </cell>
           <cell r="M54">
-            <v>0.38682074249887466</v>
+            <v>0.4050938414636639</v>
           </cell>
           <cell r="Q54">
-            <v>-0.1894468159171615</v>
+            <v>-0.20245078944536879</v>
           </cell>
         </row>
         <row r="55">
           <cell r="H55">
-            <v>-0.57634490091114654</v>
+            <v>-0.57903681911096483</v>
           </cell>
           <cell r="J55">
-            <v>-0.39584972567051246</v>
+            <v>-0.3943306525851169</v>
           </cell>
           <cell r="M55">
-            <v>-0.20585904713356956</v>
+            <v>-0.20319232197177453</v>
           </cell>
           <cell r="Q55">
-            <v>-4.232053272803607E-2</v>
+            <v>-4.5351682239474958E-2</v>
           </cell>
         </row>
         <row r="56">
           <cell r="H56">
-            <v>-0.57634490091114654</v>
+            <v>-0.57903681911096483</v>
           </cell>
           <cell r="J56">
-            <v>-0.39584972567051246</v>
+            <v>-0.3943306525851169</v>
           </cell>
           <cell r="M56">
-            <v>-0.20585904713356956</v>
+            <v>-0.20319232197177453</v>
           </cell>
           <cell r="Q56">
-            <v>-4.232053272803607E-2</v>
+            <v>-4.5351682239474958E-2</v>
           </cell>
         </row>
         <row r="57">
           <cell r="H57">
-            <v>-0.57634490091114654</v>
+            <v>-0.57903681911096483</v>
           </cell>
           <cell r="J57">
-            <v>-0.39584972567051246</v>
+            <v>-0.3943306525851169</v>
           </cell>
           <cell r="M57">
-            <v>-0.20585904713356956</v>
+            <v>-0.20319232197177453</v>
           </cell>
           <cell r="Q57">
-            <v>-4.232053272803607E-2</v>
+            <v>-4.5351682239474958E-2</v>
           </cell>
         </row>
         <row r="58">
           <cell r="H58">
-            <v>-0.43165170650309287</v>
+            <v>-0.43045596379246831</v>
           </cell>
           <cell r="J58">
-            <v>-0.18439159511209577</v>
+            <v>-0.18915885187210035</v>
           </cell>
           <cell r="M58">
-            <v>-0.15794956039873473</v>
+            <v>-0.17100234100196271</v>
           </cell>
           <cell r="Q58">
-            <v>-0.13889887457587119</v>
+            <v>-0.14149246034975063</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="H59">
+            <v>0.1844471057264194</v>
+          </cell>
+          <cell r="I59">
+            <v>0.1844471057264194</v>
+          </cell>
+          <cell r="J59">
+            <v>0.20643155178083641</v>
+          </cell>
+          <cell r="K59">
+            <v>0.20643155178083641</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6214,8 +6238,8 @@
   </sheetPr>
   <dimension ref="B1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6283,19 +6307,19 @@
       </c>
       <c r="D5" s="33">
         <f>'[1]Auto ownership'!H53</f>
-        <v>1.1169201775500097</v>
+        <v>1.1172992162790916</v>
       </c>
       <c r="E5" s="33">
         <f>'[1]Auto ownership'!J53</f>
-        <v>-1.2581644773938045</v>
+        <v>-1.2565051850306308</v>
       </c>
       <c r="F5" s="33">
         <f>'[1]Auto ownership'!M53</f>
-        <v>-3.3920136409186741</v>
+        <v>-3.3877106944960214</v>
       </c>
       <c r="G5" s="33">
         <f>'[1]Auto ownership'!Q53</f>
-        <v>-5.3456796840622633</v>
+        <v>-5.3502031433147499</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>168</v>
@@ -6330,19 +6354,19 @@
       </c>
       <c r="D6" s="33">
         <f>'[1]Auto ownership'!H54</f>
-        <v>0.57577284999430334</v>
+        <v>0.57931801393948956</v>
       </c>
       <c r="E6" s="33">
         <f>'[1]Auto ownership'!J54</f>
-        <v>0.55366202552278654</v>
+        <v>0.56301198136124597</v>
       </c>
       <c r="F6" s="33">
         <f>'[1]Auto ownership'!M54</f>
-        <v>0.38682074249887466</v>
+        <v>0.4050938414636639</v>
       </c>
       <c r="G6" s="33">
         <f>'[1]Auto ownership'!Q54</f>
-        <v>-0.1894468159171615</v>
+        <v>-0.20245078944536879</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>170</v>
@@ -6418,17 +6442,21 @@
       <c r="C8" s="19">
         <v>0</v>
       </c>
-      <c r="D8" s="19">
-        <v>0</v>
-      </c>
-      <c r="E8" s="19">
-        <v>0</v>
-      </c>
-      <c r="F8" s="19">
-        <v>0</v>
-      </c>
-      <c r="G8" s="19">
-        <v>0</v>
+      <c r="D8" s="33">
+        <f>'[1]Auto ownership'!H59</f>
+        <v>0.1844471057264194</v>
+      </c>
+      <c r="E8" s="33">
+        <f>'[1]Auto ownership'!I59</f>
+        <v>0.1844471057264194</v>
+      </c>
+      <c r="F8" s="33">
+        <f>'[1]Auto ownership'!J59</f>
+        <v>0.20643155178083641</v>
+      </c>
+      <c r="G8" s="33">
+        <f>'[1]Auto ownership'!K59</f>
+        <v>0.20643155178083641</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>174</v>
@@ -6510,19 +6538,19 @@
       </c>
       <c r="K10" s="23">
         <f>D5</f>
-        <v>1.1169201775500097</v>
+        <v>1.1172992162790916</v>
       </c>
       <c r="L10" s="23">
         <f t="shared" ref="L10:N10" si="2">E5</f>
-        <v>-1.2581644773938045</v>
+        <v>-1.2565051850306308</v>
       </c>
       <c r="M10" s="23">
         <f t="shared" si="2"/>
-        <v>-3.3920136409186741</v>
+        <v>-3.3877106944960214</v>
       </c>
       <c r="N10" s="23">
         <f t="shared" si="2"/>
-        <v>-5.3456796840622633</v>
+        <v>-5.3502031433147499</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -6534,19 +6562,19 @@
       </c>
       <c r="D11" s="33">
         <f>'[1]Auto ownership'!H55</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="E11" s="33">
         <f>'[1]Auto ownership'!J55</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="F11" s="33">
         <f>'[1]Auto ownership'!M55</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="G11" s="33">
         <f>'[1]Auto ownership'!Q55</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>181</v>
@@ -6580,19 +6608,19 @@
       </c>
       <c r="D12" s="33">
         <f>'[1]Auto ownership'!H56</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="E12" s="33">
         <f>'[1]Auto ownership'!J56</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="F12" s="33">
         <f>'[1]Auto ownership'!M56</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="G12" s="33">
         <f>'[1]Auto ownership'!Q56</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>187</v>
@@ -6603,19 +6631,19 @@
       </c>
       <c r="K12" s="21">
         <f>K10+K11</f>
-        <v>1.1169201775500097</v>
+        <v>1.1172992162790916</v>
       </c>
       <c r="L12" s="21">
         <f>L10+L11</f>
-        <v>-1.2581644773938045</v>
+        <v>-1.2565051850306308</v>
       </c>
       <c r="M12" s="21">
         <f>M10+M11</f>
-        <v>-3.3920136409186741</v>
+        <v>-3.3877106944960214</v>
       </c>
       <c r="N12" s="21">
         <f>N10+N11</f>
-        <v>-5.3456796840622633</v>
+        <v>-5.3502031433147499</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -6627,19 +6655,19 @@
       </c>
       <c r="D13" s="33">
         <f>'[1]Auto ownership'!H57</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="E13" s="33">
         <f>'[1]Auto ownership'!J57</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="F13" s="33">
         <f>'[1]Auto ownership'!M57</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="G13" s="33">
         <f>'[1]Auto ownership'!Q57</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
@@ -6651,19 +6679,19 @@
       </c>
       <c r="D14" s="34">
         <f>'[1]Auto ownership'!H58</f>
-        <v>-0.43165170650309287</v>
+        <v>-0.43045596379246831</v>
       </c>
       <c r="E14" s="34">
         <f>'[1]Auto ownership'!J58</f>
-        <v>-0.18439159511209577</v>
+        <v>-0.18915885187210035</v>
       </c>
       <c r="F14" s="34">
         <f>'[1]Auto ownership'!M58</f>
-        <v>-0.15794956039873473</v>
+        <v>-0.17100234100196271</v>
       </c>
       <c r="G14" s="34">
         <f>'[1]Auto ownership'!Q58</f>
-        <v>-0.13889887457587119</v>
+        <v>-0.14149246034975063</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -6713,19 +6741,19 @@
       </c>
       <c r="D18" s="33">
         <f>K12</f>
-        <v>1.1169201775500097</v>
+        <v>1.1172992162790916</v>
       </c>
       <c r="E18" s="33">
         <f>L12</f>
-        <v>-1.2581644773938045</v>
+        <v>-1.2565051850306308</v>
       </c>
       <c r="F18" s="33">
         <f>M12</f>
-        <v>-3.3920136409186741</v>
+        <v>-3.3877106944960214</v>
       </c>
       <c r="G18" s="33">
         <f>N12</f>
-        <v>-5.3456796840622633</v>
+        <v>-5.3502031433147499</v>
       </c>
       <c r="I18" s="22" t="s">
         <v>168</v>
@@ -6760,19 +6788,19 @@
       </c>
       <c r="D19" s="33">
         <f>K25</f>
-        <v>0.57577284999430334</v>
+        <v>0.57931801393948956</v>
       </c>
       <c r="E19" s="33">
         <f>L25</f>
-        <v>0.55366202552278654</v>
+        <v>0.56301198136124597</v>
       </c>
       <c r="F19" s="33">
         <f>M25</f>
-        <v>0.38682074249887466</v>
+        <v>0.4050938414636639</v>
       </c>
       <c r="G19" s="33">
         <f>N25</f>
-        <v>-0.1894468159171615</v>
+        <v>-0.20245078944536879</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>170</v>
@@ -6851,19 +6879,19 @@
       </c>
       <c r="D21" s="33">
         <f>K61</f>
-        <v>0</v>
+        <v>0.1844471057264194</v>
       </c>
       <c r="E21" s="33">
         <f t="shared" ref="E21:G21" si="3">L61</f>
-        <v>0</v>
+        <v>0.1844471057264194</v>
       </c>
       <c r="F21" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.20643155178083641</v>
       </c>
       <c r="G21" s="33">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.20643155178083641</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>174</v>
@@ -6941,19 +6969,19 @@
       </c>
       <c r="K23" s="23">
         <f>D6</f>
-        <v>0.57577284999430334</v>
+        <v>0.57931801393948956</v>
       </c>
       <c r="L23" s="23">
         <f>E6</f>
-        <v>0.55366202552278654</v>
+        <v>0.56301198136124597</v>
       </c>
       <c r="M23" s="23">
         <f>F6</f>
-        <v>0.38682074249887466</v>
+        <v>0.4050938414636639</v>
       </c>
       <c r="N23" s="23">
         <f>G6</f>
-        <v>-0.1894468159171615</v>
+        <v>-0.20245078944536879</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
@@ -6966,19 +6994,19 @@
       </c>
       <c r="D24" s="33">
         <f>K37</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="E24" s="33">
         <f>L37</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="F24" s="33">
         <f>M37</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="G24" s="33">
         <f>N37</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>181</v>
@@ -7013,19 +7041,19 @@
       </c>
       <c r="D25" s="33">
         <f>K37</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="E25" s="33">
         <f>L37</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="F25" s="33">
         <f>M37</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="G25" s="33">
         <f>N37</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>187</v>
@@ -7036,19 +7064,19 @@
       </c>
       <c r="K25" s="21">
         <f>K23+K24</f>
-        <v>0.57577284999430334</v>
+        <v>0.57931801393948956</v>
       </c>
       <c r="L25" s="21">
         <f>L23+L24</f>
-        <v>0.55366202552278654</v>
+        <v>0.56301198136124597</v>
       </c>
       <c r="M25" s="21">
         <f>M23+M24</f>
-        <v>0.38682074249887466</v>
+        <v>0.4050938414636639</v>
       </c>
       <c r="N25" s="21">
         <f>N23+N24</f>
-        <v>-0.1894468159171615</v>
+        <v>-0.20245078944536879</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
@@ -7061,19 +7089,19 @@
       </c>
       <c r="D26" s="33">
         <f>K37</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="E26" s="33">
         <f>L37</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="F26" s="33">
         <f>M37</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="G26" s="33">
         <f>N37</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
@@ -7085,19 +7113,19 @@
       </c>
       <c r="D27" s="34">
         <f>K49</f>
-        <v>-0.43165170650309287</v>
+        <v>-0.43045596379246831</v>
       </c>
       <c r="E27" s="34">
         <f t="shared" ref="E27:G27" si="4">L49</f>
-        <v>-0.18439159511209577</v>
+        <v>-0.18915885187210035</v>
       </c>
       <c r="F27" s="34">
         <f t="shared" si="4"/>
-        <v>-0.15794956039873473</v>
+        <v>-0.17100234100196271</v>
       </c>
       <c r="G27" s="34">
         <f t="shared" si="4"/>
-        <v>-0.13889887457587119</v>
+        <v>-0.14149246034975063</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
@@ -7236,19 +7264,19 @@
       </c>
       <c r="K35" s="23">
         <f>D12</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="L35" s="23">
         <f>E12</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="M35" s="23">
         <f>F12</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="N35" s="23">
         <f>G12</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
     </row>
     <row r="36" spans="9:14" x14ac:dyDescent="0.2">
@@ -7285,19 +7313,19 @@
       </c>
       <c r="K37" s="21">
         <f>K35+K36</f>
-        <v>-0.57634490091114654</v>
+        <v>-0.57903681911096483</v>
       </c>
       <c r="L37" s="21">
         <f>L35+L36</f>
-        <v>-0.39584972567051246</v>
+        <v>-0.3943306525851169</v>
       </c>
       <c r="M37" s="21">
         <f>M35+M36</f>
-        <v>-0.20585904713356956</v>
+        <v>-0.20319232197177453</v>
       </c>
       <c r="N37" s="21">
         <f>N35+N36</f>
-        <v>-4.232053272803607E-2</v>
+        <v>-4.5351682239474958E-2</v>
       </c>
     </row>
     <row r="41" spans="9:14" x14ac:dyDescent="0.2">
@@ -7436,19 +7464,19 @@
       </c>
       <c r="K47" s="23">
         <f>D14</f>
-        <v>-0.43165170650309287</v>
+        <v>-0.43045596379246831</v>
       </c>
       <c r="L47" s="23">
         <f>E14</f>
-        <v>-0.18439159511209577</v>
+        <v>-0.18915885187210035</v>
       </c>
       <c r="M47" s="23">
         <f>F14</f>
-        <v>-0.15794956039873473</v>
+        <v>-0.17100234100196271</v>
       </c>
       <c r="N47" s="23">
         <f>G14</f>
-        <v>-0.13889887457587119</v>
+        <v>-0.14149246034975063</v>
       </c>
     </row>
     <row r="48" spans="9:14" x14ac:dyDescent="0.2">
@@ -7485,19 +7513,19 @@
       </c>
       <c r="K49" s="21">
         <f>K47+K48</f>
-        <v>-0.43165170650309287</v>
+        <v>-0.43045596379246831</v>
       </c>
       <c r="L49" s="21">
         <f>L47+L48</f>
-        <v>-0.18439159511209577</v>
+        <v>-0.18915885187210035</v>
       </c>
       <c r="M49" s="21">
         <f>M47+M48</f>
-        <v>-0.15794956039873473</v>
+        <v>-0.17100234100196271</v>
       </c>
       <c r="N49" s="21">
         <f>N47+N48</f>
-        <v>-0.13889887457587119</v>
+        <v>-0.14149246034975063</v>
       </c>
     </row>
     <row r="52" spans="9:14" x14ac:dyDescent="0.2">
@@ -7639,19 +7667,19 @@
       </c>
       <c r="K59" s="23">
         <f>D8</f>
-        <v>0</v>
+        <v>0.1844471057264194</v>
       </c>
       <c r="L59" s="23">
         <f>E8</f>
-        <v>0</v>
+        <v>0.1844471057264194</v>
       </c>
       <c r="M59" s="23">
         <f>F8</f>
-        <v>0</v>
+        <v>0.20643155178083641</v>
       </c>
       <c r="N59" s="23">
         <f>G8</f>
-        <v>0</v>
+        <v>0.20643155178083641</v>
       </c>
     </row>
     <row r="60" spans="9:14" x14ac:dyDescent="0.2">
@@ -7688,23 +7716,31 @@
       </c>
       <c r="K61" s="21">
         <f>K59+K60</f>
-        <v>0</v>
+        <v>0.1844471057264194</v>
       </c>
       <c r="L61" s="21">
         <f>L59+L60</f>
-        <v>0</v>
+        <v>0.1844471057264194</v>
       </c>
       <c r="M61" s="21">
         <f>M59+M60</f>
-        <v>0</v>
+        <v>0.20643155178083641</v>
       </c>
       <c r="N61" s="21">
         <f>N59+N60</f>
-        <v>0</v>
+        <v>0.20643155178083641</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5:G6">
+    <cfRule type="cellIs" dxfId="11" priority="11" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:G14">
     <cfRule type="cellIs" dxfId="9" priority="9" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7712,7 +7748,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:G14">
+  <conditionalFormatting sqref="D18:G19">
     <cfRule type="cellIs" dxfId="7" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7720,7 +7756,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18:G19">
+  <conditionalFormatting sqref="D24:G27">
     <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7728,7 +7764,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:G27">
+  <conditionalFormatting sqref="D21:G21">
     <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -7736,7 +7772,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21:G21">
+  <conditionalFormatting sqref="D8:G8">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>